<commit_message>
More testing based, now to make the calculations per block and not per row
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,79 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennc\Desktop\pythonShenanigens\python_excel_read_write\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennc\Desktop\S5\Z-Z-GitHub\pythonShenanigens\python_excel_read_write\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD5D82D-C6D2-4BE8-A46D-71FBB7304987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5C8AE0-CE19-4995-9E2C-8DBDCAE5165D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="3228" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>23.3</t>
-  </si>
-  <si>
-    <t>23.5</t>
-  </si>
-  <si>
-    <t>23.4</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>23.45</t>
-  </si>
-  <si>
-    <t>23.34</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>23.44</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -92,15 +67,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,61 +412,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="B1" s="3">
+        <v>32.979999999999997</v>
+      </c>
+      <c r="C1" s="2">
+        <v>36.51</v>
+      </c>
+      <c r="D1" s="1">
+        <v>33.65</v>
+      </c>
+      <c r="E1" s="3">
+        <v>33.65</v>
+      </c>
+      <c r="F1" s="2">
+        <v>37.01</v>
+      </c>
+      <c r="G1" s="1">
+        <v>33.79</v>
+      </c>
+      <c r="H1" s="3">
+        <v>34.81</v>
+      </c>
+      <c r="I1" s="2">
+        <v>40.22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="B2" s="6">
+        <v>33.61</v>
+      </c>
+      <c r="C2" s="4">
+        <v>36.04</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33.47</v>
+      </c>
+      <c r="E2" s="6">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F2" s="4">
+        <v>36.43</v>
+      </c>
+      <c r="G2" s="5">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="H2" s="6">
+        <v>34.81</v>
+      </c>
+      <c r="I2" s="4">
+        <v>39.57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>35.58</v>
+      </c>
+      <c r="B3" s="3">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>39.51</v>
+      </c>
+      <c r="D3" s="1">
+        <v>35.159999999999997</v>
+      </c>
+      <c r="E3" s="3">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F3" s="2">
+        <v>39.94</v>
+      </c>
+      <c r="G3" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>37.31</v>
+      </c>
+      <c r="I3" s="2">
+        <v>43.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="C4" s="4">
+        <v>39.36</v>
+      </c>
+      <c r="D4" s="5">
+        <v>35.22</v>
+      </c>
+      <c r="E4" s="6">
+        <v>35.880000000000003</v>
+      </c>
+      <c r="F4" s="4">
+        <v>40.11</v>
+      </c>
+      <c r="G4" s="5">
+        <v>35.96</v>
+      </c>
+      <c r="H4" s="6">
+        <v>37.03</v>
+      </c>
+      <c r="I4" s="4">
+        <v>42.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>27.35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>39.729999999999997</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1">
+        <v>38.19</v>
+      </c>
+      <c r="E5" s="3">
+        <v>40.76</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1">
+        <v>39.49</v>
+      </c>
+      <c r="H5" s="3">
+        <v>41.48</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>39</v>
+      </c>
+      <c r="B6" s="6">
+        <v>39.85</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5">
+        <v>38.39</v>
+      </c>
+      <c r="E6" s="6">
+        <v>39.43</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5">
+        <v>39.67</v>
+      </c>
+      <c r="H6" s="6">
+        <v>42</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating the readme with some more files
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,54 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennc\Desktop\S5\Z-Z-GitHub\pythonShenanigens\python_excel_read_write\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennc\Desktop\pythonShenanigens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81DB320-37C8-4343-9916-5845CE2F0212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064046C4-A035-4671-AA56-3BA794BE4AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>23.3</t>
+  </si>
+  <si>
+    <t>23.5</t>
+  </si>
+  <si>
+    <t>23.4</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>23.45</t>
+  </si>
+  <si>
+    <t>23.34</t>
+  </si>
+  <si>
+    <t>23.44</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -59,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -67,74 +92,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,173 +378,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>33.130000000000003</v>
-      </c>
-      <c r="B1" s="3">
-        <v>32.979999999999997</v>
-      </c>
-      <c r="C1" s="2">
-        <v>36.51</v>
-      </c>
-      <c r="D1" s="1">
-        <v>33.65</v>
-      </c>
-      <c r="E1" s="3">
-        <v>33.65</v>
-      </c>
-      <c r="F1" s="2">
-        <v>37.01</v>
-      </c>
-      <c r="G1" s="1">
-        <v>33.79</v>
-      </c>
-      <c r="H1" s="3">
-        <v>34.81</v>
-      </c>
-      <c r="I1" s="2">
-        <v>40.22</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="B2" s="6">
-        <v>33.61</v>
-      </c>
-      <c r="C2" s="4">
-        <v>36.04</v>
-      </c>
-      <c r="D2" s="5">
-        <v>33.47</v>
-      </c>
-      <c r="E2" s="6">
-        <v>34.479999999999997</v>
-      </c>
-      <c r="F2" s="4">
-        <v>36.43</v>
-      </c>
-      <c r="G2" s="5">
-        <v>34.770000000000003</v>
-      </c>
-      <c r="H2" s="6">
-        <v>34.81</v>
-      </c>
-      <c r="I2" s="4">
-        <v>39.57</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>35.58</v>
-      </c>
-      <c r="B3" s="3">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="C3" s="2">
-        <v>39.51</v>
-      </c>
-      <c r="D3" s="1">
-        <v>35.159999999999997</v>
-      </c>
-      <c r="E3" s="3">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="F3" s="2">
-        <v>39.94</v>
-      </c>
-      <c r="G3" s="1">
-        <v>36.4</v>
-      </c>
-      <c r="H3" s="3">
-        <v>37.31</v>
-      </c>
-      <c r="I3" s="2">
-        <v>43.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6">
-        <v>35.950000000000003</v>
-      </c>
-      <c r="C4" s="4">
-        <v>39.36</v>
-      </c>
-      <c r="D4" s="5">
-        <v>35.22</v>
-      </c>
-      <c r="E4" s="6">
-        <v>35.880000000000003</v>
-      </c>
-      <c r="F4" s="4">
-        <v>40.11</v>
-      </c>
-      <c r="G4" s="5">
-        <v>35.96</v>
-      </c>
-      <c r="H4" s="6">
-        <v>37.03</v>
-      </c>
-      <c r="I4" s="4">
-        <v>42.37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>27.35</v>
-      </c>
-      <c r="B5" s="3">
-        <v>39.729999999999997</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1">
-        <v>38.19</v>
-      </c>
-      <c r="E5" s="3">
-        <v>40.76</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1">
-        <v>39.49</v>
-      </c>
-      <c r="H5" s="3">
-        <v>41.48</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>39</v>
-      </c>
-      <c r="B6" s="6">
-        <v>39.85</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5">
-        <v>38.39</v>
-      </c>
-      <c r="E6" s="6">
-        <v>39.43</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5">
-        <v>39.67</v>
-      </c>
-      <c r="H6" s="6">
-        <v>42</v>
-      </c>
-      <c r="I6" s="4"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>